<commit_message>
msz - starting multi select dropdown
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
+++ b/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3B158E-D386-4F7F-929A-5C8E6F59E87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395C1BC6-41F6-4451-822A-0022A88D2218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="636" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
@@ -207,9 +207,6 @@
     <t>id=chat_push_notification</t>
   </si>
   <si>
-    <t>id=select2-data-training_ids</t>
-  </si>
-  <si>
     <t>id=reminder_games_hours</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>id=training_ids</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,13 +876,13 @@
         <v>59</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>2</v>
@@ -890,97 +890,97 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AF3" s="4"/>
     </row>
@@ -1067,108 +1067,108 @@
         <v>13</v>
       </c>
       <c r="AB4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB5" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="AC5" s="1">
         <v>42</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
msz - completing first version msd
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
+++ b/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395C1BC6-41F6-4451-822A-0022A88D2218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A88422-427D-46DD-A16D-0FDE6DDEBDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="636" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
msz - first success mobile scrolling
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
+++ b/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E161D31-AEA5-4C4B-BC7A-FAE98AA03974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98F4CB3-A041-4F10-ABB7-9247F7A77F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="780" windowWidth="37308" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
msz - more scrolling and checkedState mobile
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
+++ b/Data/Pages/dlgProfil_pagBenachrichtigungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98F4CB3-A041-4F10-ABB7-9247F7A77F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA74B21C-D5CC-42F1-8C4E-56DE55A591DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="780" windowWidth="37308" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1020" yWindow="516" windowWidth="38676" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -262,8 +262,20 @@
     <t>//android.view.View[@text="Typ: Teilnahme am Training?"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
   </si>
   <si>
-    <r>
-      <t>//android.view.View[@text="Terminumfrage für Spielverlegung"]/parent::*/android.view.View[@text="</t>
+    <t>//android.widget.CheckBox[@resource-id="chat_push_notification"]</t>
+  </si>
+  <si>
+    <t>//android.widget.ListView[@resource-id="select2-training_ids-container"]</t>
+  </si>
+  <si>
+    <t>//android.widget.EditText[@resource-id="reminder_games_hours"]</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@text="Speichern"]</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Terminumfrage für Spielverlegung"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -287,11 +299,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Terminumfrage für Spielverlegung"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Bestätigung der Spielverlegung"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Terminumfrage für Spielverlegung"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Bestätigung der Spielverlegung"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -315,11 +327,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Bestätigung der Spielverlegung"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Ersatzanfrage an dich gestellt?"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Bestätigung der Spielverlegung"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Ersatz erfolgreich für dich gefunden"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -343,11 +355,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Ersatzanfrage an dich gestellt?"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Ersatz erfolgreich für dich gefunden"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Ersatz erfolgreich für dich gefunden"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Neues Mannschaftsspiel angelegt"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -371,11 +383,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Ersatz erfolgreich für dich gefunden"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Neues Mannschaftsspiel angelegt"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Neues Mannschaftsspiel angelegt"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Einladung für Vereinstermin"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -399,11 +411,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Neues Mannschaftsspiel angelegt"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Einladung für Vereinstermin"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Einladung für Vereinstermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Erinnerung an Spieltermin"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -427,11 +439,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Einladung für Vereinstermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Erinnerung an Spieltermin"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Erinnerung an Spieltermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Mannschaftsspiel zugeordnet"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -455,11 +467,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Erinnerung an Spieltermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Mannschaftsspiel zugeordnet"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Mannschaftsspiel zugeordnet"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Erinnerung an ungelesene Nachrichten im Chat"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -483,11 +495,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Mannschaftsspiel zugeordnet"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Erinnerung an ungelesene Nachrichten im Chat"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Erinnerung an ungelesene Nachrichten im Chat"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Neue Nachricht im Training, Spiel oder Vereinstermin"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -511,11 +523,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Erinnerung an ungelesene Nachrichten im Chat"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Neue Nachricht im Training, Spiel oder Vereinstermin"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Neue Nachricht im Training, Spiel oder Vereinstermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Benachrichtigung bei Trainingsausfall"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -539,11 +551,11 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Neue Nachricht im Training, Spiel oder Vereinstermin"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <r>
-      <t>//android.view.View[@text="Benachrichtigung bei Trainingsausfall"]/parent::*/android.view.View[@text="</t>
+    <t>//android.view.View[@text="Typ: Benachrichtigung bei Trainingsausfall"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
+  </si>
+  <si>
+    <r>
+      <t>//android.view.View[@text="Typ: Ersatzanfrage an dich gestellt"]/parent::*/android.view.View[@text="</t>
     </r>
     <r>
       <rPr>
@@ -567,19 +579,7 @@
     </r>
   </si>
   <si>
-    <t>//android.view.View[@text="Benachrichtigung bei Trainingsausfall"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
-  </si>
-  <si>
-    <t>//android.widget.CheckBox[@resource-id="chat_push_notification"]</t>
-  </si>
-  <si>
-    <t>//android.widget.ListView[@resource-id="select2-training_ids-container"]</t>
-  </si>
-  <si>
-    <t>//android.widget.EditText[@resource-id="reminder_games_hours"]</t>
-  </si>
-  <si>
-    <t>//android.widget.Button[@text="Speichern"]</t>
+    <t>//android.view.View[@text="Typ: Ersatzanfrage an dich gestellt"]/parent::*/android.view.View[@text="✉️ E-Mail:"]/android.widget.CheckBox</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1052,7 +1052,7 @@
     <col min="23" max="23" width="32.5546875" style="1" customWidth="1"/>
     <col min="24" max="24" width="24.44140625" style="1" customWidth="1"/>
     <col min="25" max="25" width="26.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.21875" style="1" customWidth="1"/>
     <col min="27" max="27" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="28.44140625" style="1" customWidth="1"/>
     <col min="29" max="29" width="16.33203125" style="1" customWidth="1"/>
@@ -1159,82 +1159,82 @@
         <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="AA2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="AB2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="AC2" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="4" customFormat="1">

</xml_diff>